<commit_message>
Updated stats and predictions 6/9.
</commit_message>
<xml_diff>
--- a/Projections/results.xlsx
+++ b/Projections/results.xlsx
@@ -433,13 +433,13 @@
         <v>3.078159433622178</v>
       </c>
       <c r="C2">
-        <v>2.096170510470295</v>
+        <v>1.694062797813139</v>
       </c>
       <c r="D2">
         <v>0.930906765969532</v>
       </c>
       <c r="E2">
-        <v>0.6600842926129172</v>
+        <v>0.742319372979656</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -450,13 +450,13 @@
         <v>3.078159433622178</v>
       </c>
       <c r="C3">
-        <v>2.944000023941405</v>
+        <v>2.225099032184885</v>
       </c>
       <c r="D3">
         <v>0.9262683743297593</v>
       </c>
       <c r="E3">
-        <v>0.3295079416440092</v>
+        <v>0.5554491472675398</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -467,13 +467,13 @@
         <v>3.078159433622178</v>
       </c>
       <c r="C4">
-        <v>2.605968895506064</v>
+        <v>1.940739869809948</v>
       </c>
       <c r="D4">
         <v>0.9515513183991507</v>
       </c>
       <c r="E4">
-        <v>0.4746406387180462</v>
+        <v>0.6618126070274846</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -484,13 +484,13 @@
         <v>3.078159433622178</v>
       </c>
       <c r="C5">
-        <v>2.667530053473584</v>
+        <v>2.029920287197169</v>
       </c>
       <c r="D5">
-        <v>0.9881621749363163</v>
+        <v>0.9884782555672129</v>
       </c>
       <c r="E5">
-        <v>0.4495261891644182</v>
+        <v>0.6300178890845086</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -501,13 +501,13 @@
         <v>3.078159433622178</v>
       </c>
       <c r="C6">
-        <v>2.701446279563617</v>
+        <v>2.171775041616835</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0.4354392372857744</v>
+        <v>0.5765009566294313</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -518,13 +518,13 @@
         <v>3.078159433622178</v>
       </c>
       <c r="C7">
-        <v>2.81452404999533</v>
+        <v>2.178618141920127</v>
       </c>
       <c r="D7">
-        <v>0.9148817602002632</v>
+        <v>0.9170390054603687</v>
       </c>
       <c r="E7">
-        <v>0.3871870307453771</v>
+        <v>0.5738279245335569</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -535,13 +535,13 @@
         <v>3.078159433622178</v>
       </c>
       <c r="C8">
-        <v>2.57303811836872</v>
+        <v>2.0469229793699</v>
       </c>
       <c r="D8">
-        <v>0.9824465158082911</v>
+        <v>0.9821102070623208</v>
       </c>
       <c r="E8">
-        <v>0.4878343354973976</v>
+        <v>0.6237939624380013</v>
       </c>
     </row>
   </sheetData>
@@ -579,13 +579,13 @@
         <v>9.344332308850889</v>
       </c>
       <c r="C2">
-        <v>9.777566963086064</v>
+        <v>15.01932178290843</v>
       </c>
       <c r="D2">
         <v>0.8877208431736233</v>
       </c>
       <c r="E2">
-        <v>0.2114037676806839</v>
+        <v>-1.01570273264918</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -596,13 +596,13 @@
         <v>9.344332308850889</v>
       </c>
       <c r="C3">
-        <v>9.340354089340108</v>
+        <v>6.683836766917238</v>
       </c>
       <c r="D3">
         <v>0.9398297403551975</v>
       </c>
       <c r="E3">
-        <v>0.280352566568695</v>
+        <v>0.6008119695625709</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -613,13 +613,13 @@
         <v>9.344332308850889</v>
       </c>
       <c r="C4">
-        <v>10.35974420587853</v>
+        <v>8.169039967069054</v>
       </c>
       <c r="D4">
         <v>0.8675974040093468</v>
       </c>
       <c r="E4">
-        <v>0.1146985724980872</v>
+        <v>0.4036957806847478</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -630,13 +630,13 @@
         <v>9.344332308850889</v>
       </c>
       <c r="C5">
-        <v>6.316041032913083</v>
+        <v>5.509507065597373</v>
       </c>
       <c r="D5">
-        <v>0.9912342059413729</v>
+        <v>0.9911188452018577</v>
       </c>
       <c r="E5">
-        <v>0.6709340201930153</v>
+        <v>0.7287615029017056</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -647,13 +647,13 @@
         <v>9.344332308850889</v>
       </c>
       <c r="C6">
-        <v>16.11502557719333</v>
+        <v>6.505615417033987</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>-1.142175747546689</v>
+        <v>0.6218164685608235</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -664,13 +664,13 @@
         <v>9.344332308850889</v>
       </c>
       <c r="C7">
-        <v>6.251546167056097</v>
+        <v>6.202958542276117</v>
       </c>
       <c r="D7">
-        <v>0.9161980584826135</v>
+        <v>0.9050747766293435</v>
       </c>
       <c r="E7">
-        <v>0.6776200783664436</v>
+        <v>0.6561859678006043</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -681,13 +681,13 @@
         <v>9.344332308850889</v>
       </c>
       <c r="C8">
-        <v>6.813728748250348</v>
+        <v>5.906910872072573</v>
       </c>
       <c r="D8">
-        <v>0.9869277822578379</v>
+        <v>0.9890687624604397</v>
       </c>
       <c r="E8">
-        <v>0.6170317406453067</v>
+        <v>0.6882211315531173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating 2021 statistics and projections for application
</commit_message>
<xml_diff>
--- a/Projections/results.xlsx
+++ b/Projections/results.xlsx
@@ -433,13 +433,13 @@
         <v>3.078159433622178</v>
       </c>
       <c r="C2">
-        <v>1.694062797813139</v>
+        <v>4.443236247967362</v>
       </c>
       <c r="D2">
         <v>0.930906765969532</v>
       </c>
       <c r="E2">
-        <v>0.742319372979656</v>
+        <v>-17.06722924051244</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -450,13 +450,13 @@
         <v>3.078159433622178</v>
       </c>
       <c r="C3">
-        <v>2.225099032184885</v>
+        <v>3.927950448455748</v>
       </c>
       <c r="D3">
         <v>0.9262683743297593</v>
       </c>
       <c r="E3">
-        <v>0.5554491472675398</v>
+        <v>-13.11967645362222</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -467,13 +467,13 @@
         <v>3.078159433622178</v>
       </c>
       <c r="C4">
-        <v>1.940739869809948</v>
+        <v>4.177346225815146</v>
       </c>
       <c r="D4">
         <v>0.9515513183991507</v>
       </c>
       <c r="E4">
-        <v>0.6618126070274846</v>
+        <v>-14.96958711751675</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -484,13 +484,13 @@
         <v>3.078159433622178</v>
       </c>
       <c r="C5">
-        <v>2.029920287197169</v>
+        <v>4.00401819782806</v>
       </c>
       <c r="D5">
-        <v>0.9884782555672129</v>
+        <v>0.9884672369025292</v>
       </c>
       <c r="E5">
-        <v>0.6300178890845086</v>
+        <v>-13.67184835148691</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -501,13 +501,13 @@
         <v>3.078159433622178</v>
       </c>
       <c r="C6">
-        <v>2.171775041616835</v>
+        <v>4.260782067575361</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0.5765009566294313</v>
+        <v>-15.6138921449346</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -518,13 +518,13 @@
         <v>3.078159433622178</v>
       </c>
       <c r="C7">
-        <v>2.178618141920127</v>
+        <v>3.924361314618307</v>
       </c>
       <c r="D7">
-        <v>0.9170390054603687</v>
+        <v>0.9175794647558174</v>
       </c>
       <c r="E7">
-        <v>0.5738279245335569</v>
+        <v>-13.09388475581119</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -535,13 +535,13 @@
         <v>3.078159433622178</v>
       </c>
       <c r="C8">
-        <v>2.0469229793699</v>
+        <v>3.98931807735444</v>
       </c>
       <c r="D8">
-        <v>0.9821102070623208</v>
+        <v>0.9846448435433534</v>
       </c>
       <c r="E8">
-        <v>0.6237939624380013</v>
+        <v>-13.5643153613973</v>
       </c>
     </row>
   </sheetData>
@@ -579,13 +579,13 @@
         <v>9.344332308850889</v>
       </c>
       <c r="C2">
-        <v>15.01932178290843</v>
+        <v>32.39192243400829</v>
       </c>
       <c r="D2">
         <v>0.8877208431736233</v>
       </c>
       <c r="E2">
-        <v>-1.01570273264918</v>
+        <v>-327.4602300122007</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -596,13 +596,13 @@
         <v>9.344332308850889</v>
       </c>
       <c r="C3">
-        <v>6.683836766917238</v>
+        <v>9.352564995263009</v>
       </c>
       <c r="D3">
         <v>0.9398297403551975</v>
       </c>
       <c r="E3">
-        <v>0.6008119695625709</v>
+        <v>-26.38235616466474</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -613,13 +613,13 @@
         <v>9.344332308850889</v>
       </c>
       <c r="C4">
-        <v>8.169039967069054</v>
+        <v>7.807376003184183</v>
       </c>
       <c r="D4">
         <v>0.8675974040093468</v>
       </c>
       <c r="E4">
-        <v>0.4036957806847478</v>
+        <v>-18.08180863123216</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -630,13 +630,13 @@
         <v>9.344332308850889</v>
       </c>
       <c r="C5">
-        <v>5.509507065597373</v>
+        <v>11.47327868378975</v>
       </c>
       <c r="D5">
-        <v>0.9911188452018577</v>
+        <v>0.9913980763381751</v>
       </c>
       <c r="E5">
-        <v>0.7287615029017056</v>
+        <v>-40.20827455014338</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -647,13 +647,13 @@
         <v>9.344332308850889</v>
       </c>
       <c r="C6">
-        <v>6.505615417033987</v>
+        <v>22.59497503356168</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0.6218164685608235</v>
+        <v>-158.8207177224199</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -664,13 +664,13 @@
         <v>9.344332308850889</v>
       </c>
       <c r="C7">
-        <v>6.202958542276117</v>
+        <v>10.64354763602054</v>
       </c>
       <c r="D7">
-        <v>0.9050747766293435</v>
+        <v>0.913653446242111</v>
       </c>
       <c r="E7">
-        <v>0.6561859678006043</v>
+        <v>-34.46354624278319</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -681,13 +681,13 @@
         <v>9.344332308850889</v>
       </c>
       <c r="C8">
-        <v>5.906910872072573</v>
+        <v>11.523215889036</v>
       </c>
       <c r="D8">
-        <v>0.9890687624604397</v>
+        <v>0.9878060360374233</v>
       </c>
       <c r="E8">
-        <v>0.6882211315531173</v>
+        <v>-40.56777150708511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>